<commit_message>
Updated Journal and Gantt Chart
.
</commit_message>
<xml_diff>
--- a/Project Gantt Chart.xlsx
+++ b/Project Gantt Chart.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>Character Development Research</t>
   </si>
@@ -226,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,6 +273,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -558,7 +564,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -792,6 +798,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1059,7 +1068,7 @@
   <dimension ref="B2:BQ26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G7" sqref="G7:AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1323,10 +1332,10 @@
       <c r="F9" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="78">
         <v>42674</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="78">
         <v>42681</v>
       </c>
       <c r="I9" s="7">
@@ -1454,8 +1463,8 @@
       <c r="E10" s="41">
         <v>42674</v>
       </c>
-      <c r="F10" s="40" t="s">
-        <v>18</v>
+      <c r="F10" s="40">
+        <v>2</v>
       </c>
       <c r="G10" s="76"/>
       <c r="H10" s="77"/>
@@ -1532,8 +1541,8 @@
       <c r="D11" s="44">
         <v>1</v>
       </c>
-      <c r="E11" s="45" t="s">
-        <v>18</v>
+      <c r="E11" s="45">
+        <v>42688</v>
       </c>
       <c r="F11" s="44" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Commit up to Pathfinding Code Creation
All work up to pathfinding code creation, but before pathfinding
testing.
</commit_message>
<xml_diff>
--- a/Project Gantt Chart.xlsx
+++ b/Project Gantt Chart.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>Character Development Research</t>
   </si>
@@ -564,7 +564,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -754,6 +754,9 @@
     <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="8" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -799,7 +802,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="8" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="8" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180"/>
     </xf>
   </cellXfs>
@@ -1067,8 +1070,8 @@
   </sheetPr>
   <dimension ref="B2:BQ26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:AG7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AO11" sqref="AO11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1085,13 +1088,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:69" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -1118,11 +1121,11 @@
       <c r="AD2" s="6"/>
     </row>
     <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
@@ -1157,11 +1160,11 @@
       <c r="AL3" s="12"/>
     </row>
     <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
       <c r="AC4" s="17"/>
       <c r="AD4" s="17"/>
       <c r="AE4" s="17"/>
@@ -1198,35 +1201,35 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="73"/>
-      <c r="R7" s="73"/>
-      <c r="S7" s="73"/>
-      <c r="T7" s="73"/>
-      <c r="U7" s="73"/>
-      <c r="V7" s="73"/>
-      <c r="W7" s="73"/>
-      <c r="X7" s="73"/>
-      <c r="Y7" s="73"/>
-      <c r="Z7" s="73"/>
-      <c r="AA7" s="73"/>
-      <c r="AB7" s="73"/>
-      <c r="AC7" s="73"/>
-      <c r="AD7" s="73"/>
-      <c r="AE7" s="73"/>
-      <c r="AF7" s="73"/>
-      <c r="AG7" s="73"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="74"/>
+      <c r="X7" s="74"/>
+      <c r="Y7" s="74"/>
+      <c r="Z7" s="74"/>
+      <c r="AA7" s="74"/>
+      <c r="AB7" s="74"/>
+      <c r="AC7" s="74"/>
+      <c r="AD7" s="74"/>
+      <c r="AE7" s="74"/>
+      <c r="AF7" s="74"/>
+      <c r="AG7" s="74"/>
     </row>
     <row r="8" spans="2:69" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="19"/>
@@ -1332,34 +1335,34 @@
       <c r="F9" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="78">
+      <c r="G9" s="63">
         <v>42674</v>
       </c>
-      <c r="H9" s="78">
+      <c r="H9" s="63">
         <v>42681</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="63">
         <v>42688</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="63">
         <v>42695</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="63">
         <v>42702</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="63">
         <v>42709</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="79">
         <v>42716</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="79">
         <v>42723</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="79">
         <v>42730</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P9" s="79">
         <v>42371</v>
       </c>
       <c r="Q9" s="7">
@@ -1466,17 +1469,17 @@
       <c r="F10" s="40">
         <v>2</v>
       </c>
-      <c r="G10" s="76"/>
-      <c r="H10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="78"/>
       <c r="I10" s="22"/>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
-      <c r="N10" s="65" t="s">
+      <c r="N10" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="66"/>
+      <c r="O10" s="67"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="20"/>
@@ -1544,8 +1547,8 @@
       <c r="E11" s="45">
         <v>42688</v>
       </c>
-      <c r="F11" s="44" t="s">
-        <v>18</v>
+      <c r="F11" s="44">
+        <v>1</v>
       </c>
       <c r="G11" s="30"/>
       <c r="H11" s="31"/>
@@ -1554,8 +1557,8 @@
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
-      <c r="N11" s="67"/>
-      <c r="O11" s="68"/>
+      <c r="N11" s="68"/>
+      <c r="O11" s="69"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
@@ -1620,11 +1623,11 @@
       <c r="D12" s="48">
         <v>1</v>
       </c>
-      <c r="E12" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="49" t="s">
-        <v>18</v>
+      <c r="E12" s="47">
+        <v>42695</v>
+      </c>
+      <c r="F12" s="49">
+        <v>1</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -1633,8 +1636,8 @@
       <c r="K12" s="22"/>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="68"/>
+      <c r="N12" s="68"/>
+      <c r="O12" s="69"/>
       <c r="P12" s="20"/>
       <c r="Q12" s="20"/>
       <c r="R12" s="20"/>
@@ -1699,11 +1702,11 @@
       <c r="D13" s="51">
         <v>1</v>
       </c>
-      <c r="E13" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="44" t="s">
-        <v>18</v>
+      <c r="E13" s="43">
+        <v>42702</v>
+      </c>
+      <c r="F13" s="44">
+        <v>1</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -1712,8 +1715,8 @@
       <c r="K13" s="36"/>
       <c r="L13" s="23"/>
       <c r="M13" s="24"/>
-      <c r="N13" s="67"/>
-      <c r="O13" s="68"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="69"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
@@ -1778,10 +1781,10 @@
       <c r="D14" s="48">
         <v>2</v>
       </c>
-      <c r="E14" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="49" t="s">
+      <c r="E14" s="53">
+        <v>42709</v>
+      </c>
+      <c r="F14" s="47" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="20"/>
@@ -1789,10 +1792,10 @@
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
       <c r="K14" s="32"/>
-      <c r="L14" s="74"/>
-      <c r="M14" s="75"/>
-      <c r="N14" s="69"/>
-      <c r="O14" s="68"/>
+      <c r="L14" s="75"/>
+      <c r="M14" s="76"/>
+      <c r="N14" s="70"/>
+      <c r="O14" s="69"/>
       <c r="P14" s="25"/>
       <c r="Q14" s="25"/>
       <c r="R14" s="20"/>
@@ -1857,7 +1860,7 @@
       <c r="D15" s="51">
         <v>2</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="43" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="44" t="s">
@@ -1870,10 +1873,10 @@
       <c r="K15" s="8"/>
       <c r="L15" s="30"/>
       <c r="M15" s="30"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="74"/>
-      <c r="Q15" s="75"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="70"/>
+      <c r="P15" s="75"/>
+      <c r="Q15" s="76"/>
       <c r="R15" s="23"/>
       <c r="S15" s="24"/>
       <c r="T15" s="8"/>
@@ -1949,12 +1952,12 @@
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="68"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="69"/>
       <c r="P16" s="33"/>
       <c r="Q16" s="32"/>
-      <c r="R16" s="74"/>
-      <c r="S16" s="75"/>
+      <c r="R16" s="75"/>
+      <c r="S16" s="76"/>
       <c r="T16" s="22"/>
       <c r="U16" s="25"/>
       <c r="V16" s="20"/>
@@ -2028,14 +2031,14 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
-      <c r="N17" s="67"/>
-      <c r="O17" s="68"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="69"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="30"/>
       <c r="S17" s="31"/>
-      <c r="T17" s="74"/>
-      <c r="U17" s="75"/>
+      <c r="T17" s="75"/>
+      <c r="U17" s="76"/>
       <c r="V17" s="23"/>
       <c r="W17" s="8"/>
       <c r="X17" s="8"/>
@@ -2107,8 +2110,8 @@
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
-      <c r="N18" s="67"/>
-      <c r="O18" s="68"/>
+      <c r="N18" s="68"/>
+      <c r="O18" s="69"/>
       <c r="P18" s="20"/>
       <c r="Q18" s="20"/>
       <c r="R18" s="20"/>
@@ -2186,8 +2189,8 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
-      <c r="N19" s="67"/>
-      <c r="O19" s="68"/>
+      <c r="N19" s="68"/>
+      <c r="O19" s="69"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
@@ -2195,8 +2198,8 @@
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
       <c r="V19" s="31"/>
-      <c r="W19" s="74"/>
-      <c r="X19" s="75"/>
+      <c r="W19" s="75"/>
+      <c r="X19" s="76"/>
       <c r="Y19" s="23"/>
       <c r="Z19" s="24"/>
       <c r="AA19" s="8"/>
@@ -2265,8 +2268,8 @@
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
-      <c r="N20" s="67"/>
-      <c r="O20" s="68"/>
+      <c r="N20" s="68"/>
+      <c r="O20" s="69"/>
       <c r="P20" s="20"/>
       <c r="Q20" s="20"/>
       <c r="R20" s="20"/>
@@ -2276,8 +2279,8 @@
       <c r="V20" s="20"/>
       <c r="W20" s="33"/>
       <c r="X20" s="32"/>
-      <c r="Y20" s="74"/>
-      <c r="Z20" s="75"/>
+      <c r="Y20" s="75"/>
+      <c r="Z20" s="76"/>
       <c r="AA20" s="22"/>
       <c r="AB20" s="20"/>
       <c r="AC20" s="21"/>
@@ -2344,8 +2347,8 @@
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
-      <c r="N21" s="67"/>
-      <c r="O21" s="68"/>
+      <c r="N21" s="68"/>
+      <c r="O21" s="69"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
@@ -2423,8 +2426,8 @@
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
-      <c r="N22" s="67"/>
-      <c r="O22" s="68"/>
+      <c r="N22" s="68"/>
+      <c r="O22" s="69"/>
       <c r="P22" s="20"/>
       <c r="Q22" s="20"/>
       <c r="R22" s="20"/>
@@ -2437,8 +2440,8 @@
       <c r="Y22" s="20"/>
       <c r="Z22" s="20"/>
       <c r="AA22" s="32"/>
-      <c r="AB22" s="74"/>
-      <c r="AC22" s="75"/>
+      <c r="AB22" s="75"/>
+      <c r="AC22" s="76"/>
       <c r="AD22" s="27"/>
       <c r="AE22" s="21"/>
       <c r="AF22" s="21"/>
@@ -2502,8 +2505,8 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
-      <c r="N23" s="67"/>
-      <c r="O23" s="68"/>
+      <c r="N23" s="68"/>
+      <c r="O23" s="69"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
@@ -2581,8 +2584,8 @@
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
-      <c r="N24" s="67"/>
-      <c r="O24" s="68"/>
+      <c r="N24" s="68"/>
+      <c r="O24" s="69"/>
       <c r="P24" s="20"/>
       <c r="Q24" s="20"/>
       <c r="R24" s="20"/>
@@ -2660,8 +2663,8 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
-      <c r="N25" s="70"/>
-      <c r="O25" s="71"/>
+      <c r="N25" s="71"/>
+      <c r="O25" s="72"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
@@ -2678,8 +2681,8 @@
       <c r="AC25" s="9"/>
       <c r="AD25" s="9"/>
       <c r="AE25" s="34"/>
-      <c r="AF25" s="63"/>
-      <c r="AG25" s="64"/>
+      <c r="AF25" s="64"/>
+      <c r="AG25" s="65"/>
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
       <c r="AJ25" s="6"/>

</xml_diff>

<commit_message>
Update up to employee coding
All updated work up to, but not including, employee coding.
</commit_message>
<xml_diff>
--- a/Project Gantt Chart.xlsx
+++ b/Project Gantt Chart.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Character Development Research</t>
   </si>
@@ -282,7 +282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -488,19 +488,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -532,6 +519,30 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -564,7 +575,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -712,9 +723,6 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
@@ -745,9 +753,6 @@
     <xf numFmtId="16" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -757,12 +762,45 @@
     <xf numFmtId="16" fontId="8" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -796,14 +834,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1071,7 +1106,7 @@
   <dimension ref="B2:BQ26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AO11" sqref="AO11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1088,13 +1123,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:69" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -1121,11 +1156,11 @@
       <c r="AD2" s="6"/>
     </row>
     <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
@@ -1160,11 +1195,11 @@
       <c r="AL3" s="12"/>
     </row>
     <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
       <c r="AC4" s="17"/>
       <c r="AD4" s="17"/>
       <c r="AE4" s="17"/>
@@ -1201,35 +1236,35 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="74" t="s">
+      <c r="G7" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="74"/>
-      <c r="T7" s="74"/>
-      <c r="U7" s="74"/>
-      <c r="V7" s="74"/>
-      <c r="W7" s="74"/>
-      <c r="X7" s="74"/>
-      <c r="Y7" s="74"/>
-      <c r="Z7" s="74"/>
-      <c r="AA7" s="74"/>
-      <c r="AB7" s="74"/>
-      <c r="AC7" s="74"/>
-      <c r="AD7" s="74"/>
-      <c r="AE7" s="74"/>
-      <c r="AF7" s="74"/>
-      <c r="AG7" s="74"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="83"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="83"/>
+      <c r="S7" s="83"/>
+      <c r="T7" s="83"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="83"/>
+      <c r="W7" s="83"/>
+      <c r="X7" s="83"/>
+      <c r="Y7" s="83"/>
+      <c r="Z7" s="83"/>
+      <c r="AA7" s="83"/>
+      <c r="AB7" s="83"/>
+      <c r="AC7" s="83"/>
+      <c r="AD7" s="83"/>
+      <c r="AE7" s="83"/>
+      <c r="AF7" s="83"/>
+      <c r="AG7" s="83"/>
     </row>
     <row r="8" spans="2:69" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="19"/>
@@ -1323,58 +1358,58 @@
       <c r="B9" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="62" t="s">
+      <c r="F9" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="63">
+      <c r="G9" s="61">
         <v>42674</v>
       </c>
-      <c r="H9" s="63">
+      <c r="H9" s="61">
         <v>42681</v>
       </c>
-      <c r="I9" s="63">
+      <c r="I9" s="61">
         <v>42688</v>
       </c>
-      <c r="J9" s="63">
+      <c r="J9" s="61">
         <v>42695</v>
       </c>
-      <c r="K9" s="63">
+      <c r="K9" s="61">
         <v>42702</v>
       </c>
-      <c r="L9" s="63">
+      <c r="L9" s="61">
         <v>42709</v>
       </c>
-      <c r="M9" s="79">
+      <c r="M9" s="61">
         <v>42716</v>
       </c>
-      <c r="N9" s="79">
+      <c r="N9" s="61">
         <v>42723</v>
       </c>
-      <c r="O9" s="79">
+      <c r="O9" s="61">
         <v>42730</v>
       </c>
-      <c r="P9" s="79">
+      <c r="P9" s="61">
         <v>42371</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="61">
         <v>42378</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R9" s="61">
         <v>42385</v>
       </c>
-      <c r="S9" s="7">
+      <c r="S9" s="61">
         <v>42392</v>
       </c>
-      <c r="T9" s="7">
+      <c r="T9" s="61">
         <v>42399</v>
       </c>
       <c r="U9" s="7">
@@ -1464,22 +1499,22 @@
         <v>2</v>
       </c>
       <c r="E10" s="41">
-        <v>42674</v>
-      </c>
-      <c r="F10" s="40">
+        <v>42679</v>
+      </c>
+      <c r="F10" s="65">
         <v>2</v>
       </c>
-      <c r="G10" s="77"/>
-      <c r="H10" s="78"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="87"/>
       <c r="I10" s="22"/>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
-      <c r="N10" s="66" t="s">
+      <c r="N10" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="67"/>
+      <c r="O10" s="76"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="20"/>
@@ -1545,20 +1580,20 @@
         <v>1</v>
       </c>
       <c r="E11" s="45">
-        <v>42688</v>
-      </c>
-      <c r="F11" s="44">
+        <v>42689</v>
+      </c>
+      <c r="F11" s="66">
         <v>1</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="62"/>
       <c r="H11" s="31"/>
       <c r="I11" s="36"/>
       <c r="J11" s="23"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
-      <c r="N11" s="68"/>
-      <c r="O11" s="69"/>
+      <c r="N11" s="77"/>
+      <c r="O11" s="78"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
@@ -1624,20 +1659,20 @@
         <v>1</v>
       </c>
       <c r="E12" s="47">
-        <v>42695</v>
-      </c>
-      <c r="F12" s="49">
+        <v>42696</v>
+      </c>
+      <c r="F12" s="67">
         <v>1</v>
       </c>
-      <c r="G12" s="20"/>
+      <c r="G12" s="63"/>
       <c r="H12" s="20"/>
       <c r="I12" s="32"/>
       <c r="J12" s="36"/>
       <c r="K12" s="22"/>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="69"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="78"/>
       <c r="P12" s="20"/>
       <c r="Q12" s="20"/>
       <c r="R12" s="20"/>
@@ -1693,30 +1728,30 @@
       <c r="BP12" s="5"/>
     </row>
     <row r="13" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="49" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="43">
         <v>42702</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="50">
         <v>1</v>
       </c>
       <c r="E13" s="43">
         <v>42702</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="66">
         <v>1</v>
       </c>
-      <c r="G13" s="8"/>
+      <c r="G13" s="64"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="31"/>
       <c r="K13" s="36"/>
       <c r="L13" s="23"/>
       <c r="M13" s="24"/>
-      <c r="N13" s="68"/>
-      <c r="O13" s="69"/>
+      <c r="N13" s="77"/>
+      <c r="O13" s="78"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
@@ -1772,30 +1807,30 @@
       <c r="BP13" s="5"/>
     </row>
     <row r="14" spans="2:69" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="53">
+      <c r="C14" s="52">
         <v>42709</v>
       </c>
       <c r="D14" s="48">
         <v>2</v>
       </c>
-      <c r="E14" s="53">
+      <c r="E14" s="52">
         <v>42709</v>
       </c>
-      <c r="F14" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="20"/>
+      <c r="F14" s="67">
+        <v>2</v>
+      </c>
+      <c r="G14" s="63"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
       <c r="K14" s="32"/>
-      <c r="L14" s="75"/>
-      <c r="M14" s="76"/>
-      <c r="N14" s="70"/>
-      <c r="O14" s="69"/>
+      <c r="L14" s="84"/>
+      <c r="M14" s="85"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="78"/>
       <c r="P14" s="25"/>
       <c r="Q14" s="25"/>
       <c r="R14" s="20"/>
@@ -1857,26 +1892,26 @@
       <c r="C15" s="43">
         <v>42371</v>
       </c>
-      <c r="D15" s="51">
+      <c r="D15" s="50">
         <v>2</v>
       </c>
-      <c r="E15" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="8"/>
+      <c r="E15" s="43">
+        <v>42738</v>
+      </c>
+      <c r="F15" s="68">
+        <v>2</v>
+      </c>
+      <c r="G15" s="64"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="30"/>
       <c r="M15" s="30"/>
-      <c r="N15" s="68"/>
-      <c r="O15" s="70"/>
-      <c r="P15" s="75"/>
-      <c r="Q15" s="76"/>
+      <c r="N15" s="77"/>
+      <c r="O15" s="79"/>
+      <c r="P15" s="84"/>
+      <c r="Q15" s="85"/>
       <c r="R15" s="23"/>
       <c r="S15" s="24"/>
       <c r="T15" s="8"/>
@@ -1933,31 +1968,31 @@
       <c r="B16" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="53">
+      <c r="C16" s="52">
         <v>42385</v>
       </c>
       <c r="D16" s="48">
         <v>2</v>
       </c>
-      <c r="E16" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="20"/>
+      <c r="E16" s="47">
+        <v>42751</v>
+      </c>
+      <c r="F16" s="69">
+        <v>2</v>
+      </c>
+      <c r="G16" s="63"/>
       <c r="H16" s="20"/>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
-      <c r="N16" s="68"/>
-      <c r="O16" s="69"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="78"/>
       <c r="P16" s="33"/>
       <c r="Q16" s="32"/>
-      <c r="R16" s="75"/>
-      <c r="S16" s="76"/>
+      <c r="R16" s="84"/>
+      <c r="S16" s="85"/>
       <c r="T16" s="22"/>
       <c r="U16" s="25"/>
       <c r="V16" s="20"/>
@@ -2015,30 +2050,30 @@
       <c r="C17" s="43">
         <v>42399</v>
       </c>
-      <c r="D17" s="51">
+      <c r="D17" s="50">
         <v>2</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="45">
+        <v>31</v>
+      </c>
+      <c r="F17" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="8"/>
+      <c r="G17" s="64"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
-      <c r="N17" s="68"/>
-      <c r="O17" s="69"/>
+      <c r="N17" s="77"/>
+      <c r="O17" s="78"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="30"/>
       <c r="S17" s="31"/>
-      <c r="T17" s="75"/>
-      <c r="U17" s="76"/>
+      <c r="T17" s="84"/>
+      <c r="U17" s="85"/>
       <c r="V17" s="23"/>
       <c r="W17" s="8"/>
       <c r="X17" s="8"/>
@@ -2091,27 +2126,27 @@
       <c r="B18" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="54">
+      <c r="C18" s="53">
         <v>42413</v>
       </c>
       <c r="D18" s="48">
         <v>1</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="49" t="s">
+      <c r="F18" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="20"/>
+      <c r="G18" s="63"/>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
-      <c r="N18" s="68"/>
-      <c r="O18" s="69"/>
+      <c r="N18" s="77"/>
+      <c r="O18" s="78"/>
       <c r="P18" s="20"/>
       <c r="Q18" s="20"/>
       <c r="R18" s="20"/>
@@ -2173,24 +2208,24 @@
       <c r="C19" s="43">
         <v>42420</v>
       </c>
-      <c r="D19" s="51">
+      <c r="D19" s="50">
         <v>2</v>
       </c>
       <c r="E19" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="44" t="s">
+      <c r="F19" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="8"/>
+      <c r="G19" s="64"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
-      <c r="N19" s="68"/>
-      <c r="O19" s="69"/>
+      <c r="N19" s="77"/>
+      <c r="O19" s="78"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
@@ -2198,8 +2233,8 @@
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
       <c r="V19" s="31"/>
-      <c r="W19" s="75"/>
-      <c r="X19" s="76"/>
+      <c r="W19" s="84"/>
+      <c r="X19" s="85"/>
       <c r="Y19" s="23"/>
       <c r="Z19" s="24"/>
       <c r="AA19" s="8"/>
@@ -2249,7 +2284,7 @@
       <c r="B20" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="53">
+      <c r="C20" s="52">
         <v>42435</v>
       </c>
       <c r="D20" s="48">
@@ -2258,18 +2293,18 @@
       <c r="E20" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="49" t="s">
+      <c r="F20" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="20"/>
+      <c r="G20" s="63"/>
       <c r="H20" s="20"/>
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
-      <c r="N20" s="68"/>
-      <c r="O20" s="69"/>
+      <c r="N20" s="77"/>
+      <c r="O20" s="78"/>
       <c r="P20" s="20"/>
       <c r="Q20" s="20"/>
       <c r="R20" s="20"/>
@@ -2279,8 +2314,8 @@
       <c r="V20" s="20"/>
       <c r="W20" s="33"/>
       <c r="X20" s="32"/>
-      <c r="Y20" s="75"/>
-      <c r="Z20" s="76"/>
+      <c r="Y20" s="84"/>
+      <c r="Z20" s="85"/>
       <c r="AA20" s="22"/>
       <c r="AB20" s="20"/>
       <c r="AC20" s="21"/>
@@ -2331,24 +2366,24 @@
       <c r="C21" s="43">
         <v>42449</v>
       </c>
-      <c r="D21" s="51">
+      <c r="D21" s="50">
         <v>1</v>
       </c>
       <c r="E21" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="8"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
-      <c r="N21" s="68"/>
-      <c r="O21" s="69"/>
+      <c r="N21" s="77"/>
+      <c r="O21" s="78"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
@@ -2407,7 +2442,7 @@
       <c r="B22" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="53">
+      <c r="C22" s="52">
         <v>42456</v>
       </c>
       <c r="D22" s="48">
@@ -2416,18 +2451,18 @@
       <c r="E22" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="49" t="s">
+      <c r="F22" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="20"/>
+      <c r="G22" s="63"/>
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
-      <c r="N22" s="68"/>
-      <c r="O22" s="69"/>
+      <c r="N22" s="77"/>
+      <c r="O22" s="78"/>
       <c r="P22" s="20"/>
       <c r="Q22" s="20"/>
       <c r="R22" s="20"/>
@@ -2440,8 +2475,8 @@
       <c r="Y22" s="20"/>
       <c r="Z22" s="20"/>
       <c r="AA22" s="32"/>
-      <c r="AB22" s="75"/>
-      <c r="AC22" s="76"/>
+      <c r="AB22" s="84"/>
+      <c r="AC22" s="85"/>
       <c r="AD22" s="27"/>
       <c r="AE22" s="21"/>
       <c r="AF22" s="21"/>
@@ -2483,30 +2518,30 @@
       <c r="BP22" s="5"/>
     </row>
     <row r="23" spans="2:68" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="43">
         <v>42470</v>
       </c>
-      <c r="D23" s="51">
+      <c r="D23" s="50">
         <v>1</v>
       </c>
       <c r="E23" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="44" t="s">
+      <c r="F23" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="8"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
-      <c r="N23" s="68"/>
-      <c r="O23" s="69"/>
+      <c r="N23" s="77"/>
+      <c r="O23" s="78"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
@@ -2562,10 +2597,10 @@
       <c r="BP23" s="5"/>
     </row>
     <row r="24" spans="2:68" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="53">
+      <c r="C24" s="52">
         <v>42477</v>
       </c>
       <c r="D24" s="48">
@@ -2574,18 +2609,18 @@
       <c r="E24" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="49" t="s">
+      <c r="F24" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="20"/>
+      <c r="G24" s="63"/>
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
-      <c r="N24" s="68"/>
-      <c r="O24" s="69"/>
+      <c r="N24" s="77"/>
+      <c r="O24" s="78"/>
       <c r="P24" s="20"/>
       <c r="Q24" s="20"/>
       <c r="R24" s="20"/>
@@ -2641,30 +2676,30 @@
       <c r="BP24" s="5"/>
     </row>
     <row r="25" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="57">
+      <c r="C25" s="56">
         <v>42484</v>
       </c>
-      <c r="D25" s="58">
+      <c r="D25" s="57">
         <v>2</v>
       </c>
-      <c r="E25" s="59" t="s">
+      <c r="E25" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="60" t="s">
+      <c r="F25" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="8"/>
+      <c r="G25" s="64"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
-      <c r="N25" s="71"/>
-      <c r="O25" s="72"/>
+      <c r="N25" s="80"/>
+      <c r="O25" s="81"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
@@ -2681,8 +2716,8 @@
       <c r="AC25" s="9"/>
       <c r="AD25" s="9"/>
       <c r="AE25" s="34"/>
-      <c r="AF25" s="64"/>
-      <c r="AG25" s="65"/>
+      <c r="AF25" s="73"/>
+      <c r="AG25" s="74"/>
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
       <c r="AJ25" s="6"/>

</xml_diff>

<commit_message>
Work up to 12th February
Added furniture sprites and code to the game. Added rotation to the
game.
</commit_message>
<xml_diff>
--- a/Project Gantt Chart.xlsx
+++ b/Project Gantt Chart.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Character Development Research</t>
   </si>
@@ -1106,7 +1106,7 @@
   <dimension ref="B2:BQ26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1412,10 +1412,10 @@
       <c r="T9" s="61">
         <v>42399</v>
       </c>
-      <c r="U9" s="7">
+      <c r="U9" s="61">
         <v>42406</v>
       </c>
-      <c r="V9" s="7">
+      <c r="V9" s="61">
         <v>42413</v>
       </c>
       <c r="W9" s="7">
@@ -2056,8 +2056,8 @@
       <c r="E17" s="45">
         <v>31</v>
       </c>
-      <c r="F17" s="68" t="s">
-        <v>18</v>
+      <c r="F17" s="68">
+        <v>2</v>
       </c>
       <c r="G17" s="64"/>
       <c r="H17" s="8"/>

</xml_diff>

<commit_message>
Work up to 21 Feb 2017
All work including second presentation
</commit_message>
<xml_diff>
--- a/Project Gantt Chart.xlsx
+++ b/Project Gantt Chart.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Character Development Research</t>
   </si>
@@ -575,7 +575,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -839,6 +839,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1106,7 +1109,7 @@
   <dimension ref="B2:BQ26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="AS10" sqref="AS10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1415,7 +1418,7 @@
       <c r="U9" s="61">
         <v>42406</v>
       </c>
-      <c r="V9" s="61">
+      <c r="V9" s="88">
         <v>42413</v>
       </c>
       <c r="W9" s="7">
@@ -2056,8 +2059,8 @@
       <c r="E17" s="45">
         <v>31</v>
       </c>
-      <c r="F17" s="68">
-        <v>2</v>
+      <c r="F17" s="68" t="s">
+        <v>18</v>
       </c>
       <c r="G17" s="64"/>
       <c r="H17" s="8"/>

</xml_diff>

<commit_message>
All work up to web deployment
.
</commit_message>
<xml_diff>
--- a/Project Gantt Chart.xlsx
+++ b/Project Gantt Chart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
@@ -575,7 +575,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -839,9 +839,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1109,7 +1106,7 @@
   <dimension ref="B2:BQ26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AS10" sqref="AS10"/>
+      <selection activeCell="Y10" sqref="Y10:Z20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1418,16 +1415,16 @@
       <c r="U9" s="61">
         <v>42406</v>
       </c>
-      <c r="V9" s="88">
+      <c r="V9" s="61">
         <v>42413</v>
       </c>
-      <c r="W9" s="7">
+      <c r="W9" s="61">
         <v>42420</v>
       </c>
-      <c r="X9" s="7">
+      <c r="X9" s="61">
         <v>42427</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="Y9" s="61">
         <v>42435</v>
       </c>
       <c r="Z9" s="7">

</xml_diff>

<commit_message>
Dissertation Write up 7500 words.
</commit_message>
<xml_diff>
--- a/Project Gantt Chart.xlsx
+++ b/Project Gantt Chart.xlsx
@@ -1106,7 +1106,7 @@
   <dimension ref="B2:BQ26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10:Z20"/>
+      <selection activeCell="AK14" sqref="AK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1427,28 +1427,28 @@
       <c r="Y9" s="61">
         <v>42435</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="Z9" s="61">
         <v>42442</v>
       </c>
-      <c r="AA9" s="7">
+      <c r="AA9" s="61">
         <v>42449</v>
       </c>
-      <c r="AB9" s="7">
+      <c r="AB9" s="61">
         <v>42456</v>
       </c>
-      <c r="AC9" s="7">
+      <c r="AC9" s="61">
         <v>42463</v>
       </c>
-      <c r="AD9" s="7">
+      <c r="AD9" s="61">
         <v>42470</v>
       </c>
-      <c r="AE9" s="7">
+      <c r="AE9" s="61">
         <v>42477</v>
       </c>
-      <c r="AF9" s="7">
+      <c r="AF9" s="61">
         <v>42484</v>
       </c>
-      <c r="AG9" s="7">
+      <c r="AG9" s="61">
         <v>42491</v>
       </c>
       <c r="AH9" s="7"/>

</xml_diff>